<commit_message>
Marked up to assignment 13
</commit_message>
<xml_diff>
--- a/assignments/2021/responses.xlsx
+++ b/assignments/2021/responses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phil/workspace/com3529/assignments/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD0F465-5794-4743-A57E-B0BFC68C2ABF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689A1CC1-565F-D849-BB50-7F455F3C27BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51600" yWindow="-2240" windowWidth="19420" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="146">
   <si>
     <t>Your name</t>
   </si>
@@ -476,6 +476,21 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>28 can mark</t>
+  </si>
+  <si>
+    <t>29 done by Tues (2 per day)</t>
+  </si>
+  <si>
+    <t>21 done by today</t>
+  </si>
+  <si>
+    <t>10 remaining over 3 days</t>
+  </si>
+  <si>
+    <t>(could be more drawn out than that)</t>
   </si>
 </sst>
 </file>
@@ -772,11 +787,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -978,16 +993,22 @@
       <c r="E14" s="4" t="s">
         <v>49</v>
       </c>
+      <c r="G14" s="8" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="6" t="s">
         <v>52</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1000,6 +1021,9 @@
       <c r="E16" s="4" t="s">
         <v>55</v>
       </c>
+      <c r="G16" s="8" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
@@ -1008,8 +1032,11 @@
       <c r="B17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="6" t="s">
         <v>58</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1022,6 +1049,9 @@
       <c r="E18" s="4" t="s">
         <v>61</v>
       </c>
+      <c r="G18" s="8" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
@@ -1033,8 +1063,11 @@
       <c r="C19" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="6" t="s">
         <v>65</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1341,7 +1374,7 @@
       </c>
       <c r="G40">
         <f>COUNTIF(G2:G39, "Yes")</f>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H40">
         <f>39-COUNTIF(H2:H39, "")</f>
@@ -1351,7 +1384,30 @@
     <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G41" s="7">
         <f>G40/38</f>
-        <v>0.28947368421052633</v>
+        <v>0.44736842105263158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G43" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G44" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G45" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G47" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1395,8 +1451,9 @@
     <hyperlink ref="E38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
     <hyperlink ref="E39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
     <hyperlink ref="B20" r:id="rId39" xr:uid="{C57EBB35-0B6B-BD4F-A10E-D1B481ED809D}"/>
+    <hyperlink ref="B15" r:id="rId40" xr:uid="{B26694FB-2F0A-5F46-9630-3556C1512D4C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId40"/>
+  <legacyDrawing r:id="rId41"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Marked up to assignment 11
</commit_message>
<xml_diff>
--- a/assignments/2021/responses.xlsx
+++ b/assignments/2021/responses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phil/workspace/com3529/assignments/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689A1CC1-565F-D849-BB50-7F455F3C27BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93359DBB-759E-D748-8E13-E76DFC30929D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51600" yWindow="-2240" windowWidth="19420" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="146">
   <si>
     <t>Your name</t>
   </si>
@@ -791,7 +791,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -968,8 +968,11 @@
       <c r="C12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="6" t="s">
         <v>43</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -982,6 +985,9 @@
       <c r="E13" s="4" t="s">
         <v>46</v>
       </c>
+      <c r="G13" s="8" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
@@ -1374,7 +1380,7 @@
       </c>
       <c r="G40">
         <f>COUNTIF(G2:G39, "Yes")</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H40">
         <f>39-COUNTIF(H2:H39, "")</f>
@@ -1384,7 +1390,7 @@
     <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G41" s="7">
         <f>G40/38</f>
-        <v>0.44736842105263158</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>